<commit_message>
Chnaged Excel read function
</commit_message>
<xml_diff>
--- a/src/resource/ParentImport.xlsx
+++ b/src/resource/ParentImport.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parag Jain\Desktop\ZippSlip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parag Jain\git\Zippslip Forms\zippslip\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12975" windowHeight="5865"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>School Id</t>
   </si>
@@ -44,62 +44,32 @@
     <t>Parent Password</t>
   </si>
   <si>
-    <t>S565661</t>
-  </si>
-  <si>
-    <t>Parent S565661</t>
-  </si>
-  <si>
-    <t>Last S565661</t>
-  </si>
-  <si>
-    <t>ParentS565661@yomail.com</t>
-  </si>
-  <si>
     <t>zippy1</t>
   </si>
   <si>
-    <t>S565662</t>
-  </si>
-  <si>
-    <t>Parent S565662</t>
-  </si>
-  <si>
-    <t>Last S565662</t>
-  </si>
-  <si>
-    <t>ParentS565662@yomail.com</t>
-  </si>
-  <si>
-    <t>S565663</t>
-  </si>
-  <si>
-    <t>Parent S565663</t>
-  </si>
-  <si>
-    <t>Last S565663</t>
-  </si>
-  <si>
-    <t>ParentS565663@yomail.com</t>
-  </si>
-  <si>
-    <t>S565664</t>
-  </si>
-  <si>
-    <t>Parent S565664</t>
-  </si>
-  <si>
-    <t>Last S565664</t>
-  </si>
-  <si>
-    <t>ParentS565664@yomail.com</t>
+    <t>Parent S565665</t>
+  </si>
+  <si>
+    <t>Last S565665</t>
+  </si>
+  <si>
+    <t>S565670</t>
+  </si>
+  <si>
+    <t>ParentS565670@yopmail.com</t>
+  </si>
+  <si>
+    <t>S565671</t>
+  </si>
+  <si>
+    <t>ParentS565671@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,14 +80,6 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,21 +99,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,11 +433,11 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +462,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -511,11 +470,11 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -526,63 +485,22 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>